<commit_message>
Add upload form tests
</commit_message>
<xml_diff>
--- a/formshare/tests/resources/forms/form01.xlsx
+++ b/formshare/tests/resources/forms/form01.xlsx
@@ -96,7 +96,7 @@
     <t xml:space="preserve">Crop</t>
   </si>
   <si>
-    <t xml:space="preserve">geopoint</t>
+    <t xml:space="preserve">geopointX</t>
   </si>
   <si>
     <t xml:space="preserve">gps</t>
@@ -294,7 +294,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>